<commit_message>
Aug 17: [FIX] Bug Fixed 'import_bill_of_materials_in_mrp'
</commit_message>
<xml_diff>
--- a/import_bill_of_materials_in_mrp/static/download/import_bom_excel.xlsx
+++ b/import_bill_of_materials_in_mrp/static/download/import_bom_excel.xlsx
@@ -86,7 +86,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -107,11 +107,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -161,7 +156,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -188,13 +183,13 @@
       <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.59"/>

</xml_diff>